<commit_message>
refactor, countdown btn, recacap
</commit_message>
<xml_diff>
--- a/src/admin/tests.xlsx
+++ b/src/admin/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dayfireacad/trainpython/src/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F0E5D4-F465-2247-AC58-14FAC592C19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221EB25F-9797-9741-8ECB-DFA3D26FB35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{A1EC0760-0569-1443-8C4C-047456B792FA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>task</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Выведи: Я знаю команду print</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>print</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>Выведи две строчки:\n1 2 3\nОдин, В программе должны обязательно присутствовать запятые</t>
   </si>
   <si>
-    <t>realdefcode</t>
-  </si>
-  <si>
     <t>rightcode</t>
   </si>
   <si>
@@ -191,6 +185,9 @@
   </si>
   <si>
     <t>defaultoutput</t>
+  </si>
+  <si>
+    <t>a=input()\nprint(int(a/3))</t>
   </si>
 </sst>
 </file>
@@ -575,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3359BBA2-D3CF-9A4D-8F52-F9BD733F6E43}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -586,19 +583,20 @@
     <col min="3" max="3" width="97.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
-    <col min="6" max="10" width="10.83203125" style="1"/>
-    <col min="11" max="11" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="89.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -607,37 +605,34 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -648,40 +643,37 @@
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1">
+      <c r="H2" s="1">
         <v>3</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -699,34 +691,31 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="H3" s="1">
         <v>2</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="J3" s="1">
+        <v>19</v>
+      </c>
       <c r="K3" s="1">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L3" s="1">
+        <v>20</v>
+      </c>
+      <c r="M3" s="1">
         <v>6</v>
       </c>
-      <c r="M3" s="1">
-        <v>20</v>
-      </c>
-      <c r="N3" s="1">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>3</v>
@@ -738,31 +727,28 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1">
+      <c r="H4" s="1">
         <v>2</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>47</v>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -774,40 +760,37 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="1">
+      <c r="H5" s="1">
         <v>3</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="K5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -825,31 +808,31 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="1">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1">
         <v>7</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="J6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="1">
+      <c r="K6" s="1">
         <v>7</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="1">
+      <c r="M6" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -861,32 +844,29 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="1" t="s">
-        <v>26</v>
+      <c r="L7" s="3"/>
+      <c r="M7" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ref="A8" si="1">A7+1</f>
         <v>7</v>
@@ -895,32 +875,32 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="1">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="1" t="s">
-        <v>28</v>
+      <c r="I8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ref="A9" si="2">A8+1</f>
         <v>8</v>
@@ -929,32 +909,32 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="1" t="s">
-        <v>28</v>
+      <c r="K9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ref="A10" si="3">A9+1</f>
         <v>9</v>
@@ -963,32 +943,29 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="1">
-        <v>2</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="1" t="s">
-        <v>51</v>
+      <c r="K10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>